<commit_message>
update libs version settings.
</commit_message>
<xml_diff>
--- a/tests/htdocs/px-files/sitemaps/sitemap.xlsx
+++ b/tests/htdocs/px-files/sitemaps/sitemap.xlsx
@@ -15,15 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
-  <si>
-    <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+  <si>
+    <t>row_definition=8&amp;row_data_start=9&amp;skip_empty_col=20&amp;version=2.0.12</t>
   </si>
   <si>
     <t>「Pickles 2」 サイトマップ</t>
   </si>
   <si>
-    <t>Exported: 2016-01-02 18:56:11</t>
+    <t>Exported: 2020-08-12 17:32:14</t>
   </si>
   <si>
     <t>ページID</t>
@@ -50,6 +50,9 @@
     <t>コンテンツファイルの格納先</t>
   </si>
   <si>
+    <t>論理構造上のパス</t>
+  </si>
+  <si>
     <t>一覧表示フラグ</t>
   </si>
   <si>
@@ -68,52 +71,64 @@
     <t>カテゴリトップフラグ</t>
   </si>
   <si>
+    <t>ロール</t>
+  </si>
+  <si>
+    <t>コンテンツの処理方法</t>
+  </si>
+  <si>
     <t>削除フラグ</t>
   </si>
   <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>title_h1</t>
+  </si>
+  <si>
+    <t>title_label</t>
+  </si>
+  <si>
+    <t>title_breadcrumb</t>
+  </si>
+  <si>
+    <t>title_full</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>logical_path</t>
+  </si>
+  <si>
+    <t>list_flg</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>orderby</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>category_top_flg</t>
+  </si>
+  <si>
     <t>role</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>title_h1</t>
-  </si>
-  <si>
-    <t>title_label</t>
-  </si>
-  <si>
-    <t>title_breadcrumb</t>
-  </si>
-  <si>
-    <t>title_full</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t>list_flg</t>
-  </si>
-  <si>
-    <t>layout</t>
-  </si>
-  <si>
-    <t>orderby</t>
-  </si>
-  <si>
-    <t>keywords</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>category_top_flg</t>
+    <t>proc_type</t>
   </si>
   <si>
     <t>**delete_flg</t>
@@ -758,13 +773,13 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="W33" sqref="W33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -782,15 +797,15 @@
     <col min="11" max="11" width="2" customWidth="true" style="0"/>
     <col min="12" max="12" width="40" customWidth="true" style="0"/>
     <col min="13" max="13" width="20" customWidth="true" style="0"/>
-    <col min="14" max="14" width="3" customWidth="true" style="0"/>
-    <col min="15" max="15" width="9" customWidth="true" style="0"/>
+    <col min="15" max="15" width="3" customWidth="true" style="0"/>
+    <col min="16" max="16" width="9" customWidth="true" style="0"/>
+    <col min="19" max="19" width="30" customWidth="true" style="0"/>
     <col min="18" max="18" width="30" customWidth="true" style="0"/>
-    <col min="17" max="17" width="30" customWidth="true" style="0"/>
-    <col min="16" max="16" width="3" customWidth="true" style="0"/>
-    <col min="19" max="19" width="3" customWidth="true" style="0"/>
+    <col min="17" max="17" width="3" customWidth="true" style="0"/>
+    <col min="20" max="20" width="3" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" customHeight="1" ht="10">
+    <row r="1" spans="1:23" customHeight="1" ht="10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,18 +829,20 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:23">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -879,13 +896,19 @@
       <c r="U7" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -893,52 +916,58 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="S8" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T8" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
+        <v>36</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -950,27 +979,29 @@
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M9" s="4"/>
-      <c r="N9" s="4">
-        <v>1</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="9"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4">
+        <v>1</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="4"/>
       <c r="R9" s="9"/>
-      <c r="S9" s="4"/>
+      <c r="S9" s="9"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="8" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
@@ -981,32 +1012,34 @@
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="M10" s="4"/>
-      <c r="N10" s="4">
-        <v>1</v>
-      </c>
-      <c r="O10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4">
+        <v>1</v>
+      </c>
       <c r="P10" s="4"/>
-      <c r="Q10" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q10" s="4"/>
       <c r="R10" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S10" s="4">
-        <v>1</v>
-      </c>
-      <c r="T10" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T10" s="4">
+        <v>1</v>
+      </c>
       <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="8" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1016,27 +1049,29 @@
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="M11" s="4"/>
-      <c r="N11" s="4">
-        <v>1</v>
-      </c>
-      <c r="O11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4">
+        <v>1</v>
+      </c>
       <c r="P11" s="4"/>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="4"/>
       <c r="R11" s="9"/>
-      <c r="S11" s="4"/>
+      <c r="S11" s="9"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -1045,27 +1080,29 @@
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="M12" s="4"/>
-      <c r="N12" s="4">
-        <v>1</v>
-      </c>
-      <c r="O12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4">
+        <v>1</v>
+      </c>
       <c r="P12" s="4"/>
-      <c r="Q12" s="9"/>
+      <c r="Q12" s="4"/>
       <c r="R12" s="9"/>
-      <c r="S12" s="4"/>
+      <c r="S12" s="9"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="4"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="8" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -1074,27 +1111,29 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="M13" s="4"/>
-      <c r="N13" s="4">
-        <v>1</v>
-      </c>
-      <c r="O13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4">
+        <v>1</v>
+      </c>
       <c r="P13" s="4"/>
-      <c r="Q13" s="9"/>
+      <c r="Q13" s="4"/>
       <c r="R13" s="9"/>
-      <c r="S13" s="4"/>
+      <c r="S13" s="9"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="8" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -1103,27 +1142,29 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="M14" s="4"/>
-      <c r="N14" s="4">
-        <v>1</v>
-      </c>
-      <c r="O14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4">
+        <v>1</v>
+      </c>
       <c r="P14" s="4"/>
-      <c r="Q14" s="9"/>
+      <c r="Q14" s="4"/>
       <c r="R14" s="9"/>
-      <c r="S14" s="4"/>
+      <c r="S14" s="9"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1132,26 +1173,28 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="M15" s="4"/>
-      <c r="N15" s="4">
-        <v>1</v>
-      </c>
-      <c r="O15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4">
+        <v>1</v>
+      </c>
       <c r="P15" s="4"/>
-      <c r="Q15" s="9"/>
+      <c r="Q15" s="4"/>
       <c r="R15" s="9"/>
-      <c r="S15" s="4"/>
+      <c r="S15" s="9"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7"/>
       <c r="D16" s="8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1161,21 +1204,23 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="M16" s="4"/>
-      <c r="N16" s="4">
-        <v>1</v>
-      </c>
-      <c r="O16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4">
+        <v>1</v>
+      </c>
       <c r="P16" s="4"/>
-      <c r="Q16" s="9"/>
+      <c r="Q16" s="4"/>
       <c r="R16" s="9"/>
-      <c r="S16" s="4"/>
+      <c r="S16" s="9"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
@@ -1186,40 +1231,42 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="4" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M17" s="4"/>
-      <c r="N17" s="4">
-        <v>1</v>
-      </c>
-      <c r="O17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4">
+        <v>1</v>
+      </c>
       <c r="P17" s="4"/>
-      <c r="Q17" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q17" s="4"/>
       <c r="R17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S17" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S17" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="8" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1229,30 +1276,32 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="M18" s="4"/>
-      <c r="N18" s="4">
-        <v>1</v>
-      </c>
-      <c r="O18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4">
+        <v>1</v>
+      </c>
       <c r="P18" s="4"/>
-      <c r="Q18" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q18" s="4"/>
       <c r="R18" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S18" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S18" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1262,30 +1311,32 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="M19" s="4"/>
-      <c r="N19" s="4">
-        <v>1</v>
-      </c>
-      <c r="O19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4">
+        <v>1</v>
+      </c>
       <c r="P19" s="4"/>
-      <c r="Q19" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q19" s="4"/>
       <c r="R19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S19" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S19" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="8" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1295,34 +1346,36 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="N20" s="4">
-        <v>1</v>
-      </c>
-      <c r="O20" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4">
+        <v>1</v>
+      </c>
       <c r="P20" s="4"/>
-      <c r="Q20" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q20" s="4"/>
       <c r="R20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S20" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S20" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1332,29 +1385,31 @@
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="M21" s="4"/>
-      <c r="N21" s="4">
-        <v>1</v>
-      </c>
-      <c r="O21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4">
+        <v>1</v>
+      </c>
       <c r="P21" s="4"/>
-      <c r="Q21" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q21" s="4"/>
       <c r="R21" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S21" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S21" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
       <c r="C22" s="8" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1365,32 +1420,34 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="M22" s="4"/>
-      <c r="N22" s="4">
-        <v>1</v>
-      </c>
-      <c r="O22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4">
+        <v>1</v>
+      </c>
       <c r="P22" s="4"/>
-      <c r="Q22" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q22" s="4"/>
       <c r="R22" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S22" s="4">
-        <v>1</v>
-      </c>
-      <c r="T22" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S22" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T22" s="4">
+        <v>1</v>
+      </c>
       <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" s="4"/>
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="8" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1400,30 +1457,32 @@
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="M23" s="4"/>
-      <c r="N23" s="4">
-        <v>1</v>
-      </c>
-      <c r="O23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4">
+        <v>1</v>
+      </c>
       <c r="P23" s="4"/>
-      <c r="Q23" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q23" s="4"/>
       <c r="R23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S23" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S23" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="V23" s="4"/>
+      <c r="W23" s="4"/>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7"/>
       <c r="D24" s="8" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1433,31 +1492,33 @@
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="M24" s="4"/>
-      <c r="N24" s="4">
-        <v>1</v>
-      </c>
-      <c r="O24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4">
+        <v>1</v>
+      </c>
       <c r="P24" s="4"/>
-      <c r="Q24" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q24" s="4"/>
       <c r="R24" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S24" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S24" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="V24" s="4"/>
+      <c r="W24" s="4"/>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" s="4"/>
       <c r="B25" s="6"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="8" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -1466,33 +1527,35 @@
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N25" s="4">
-        <v>1</v>
-      </c>
-      <c r="O25" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4">
+        <v>1</v>
+      </c>
       <c r="P25" s="4"/>
-      <c r="Q25" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q25" s="4"/>
       <c r="R25" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S25" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S25" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="1:21">
+      <c r="V25" s="4"/>
+      <c r="W25" s="4"/>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" s="4"/>
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -1501,31 +1564,33 @@
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="N26" s="4">
-        <v>1</v>
-      </c>
-      <c r="O26" s="4"/>
+        <v>77</v>
+      </c>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4">
+        <v>1</v>
+      </c>
       <c r="P26" s="4"/>
-      <c r="Q26" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q26" s="4"/>
       <c r="R26" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S26" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="V26" s="4"/>
+      <c r="W26" s="4"/>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" s="4"/>
       <c r="B27" s="6"/>
       <c r="C27" s="8" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
@@ -1536,32 +1601,34 @@
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M27" s="4"/>
-      <c r="N27" s="4">
-        <v>1</v>
-      </c>
-      <c r="O27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4">
+        <v>1</v>
+      </c>
       <c r="P27" s="4"/>
-      <c r="Q27" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q27" s="4"/>
       <c r="R27" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S27" s="4">
-        <v>1</v>
-      </c>
-      <c r="T27" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T27" s="4">
+        <v>1</v>
+      </c>
       <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" s="4"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -1571,30 +1638,32 @@
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
       <c r="L28" s="4" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="M28" s="4"/>
-      <c r="N28" s="4">
-        <v>1</v>
-      </c>
-      <c r="O28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4">
+        <v>1</v>
+      </c>
       <c r="P28" s="4"/>
-      <c r="Q28" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q28" s="4"/>
       <c r="R28" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S28" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S28" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" s="4"/>
       <c r="B29" s="6"/>
       <c r="C29" s="7"/>
       <c r="D29" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -1604,29 +1673,31 @@
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="M29" s="4"/>
-      <c r="N29" s="4">
-        <v>1</v>
-      </c>
-      <c r="O29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4">
+        <v>1</v>
+      </c>
       <c r="P29" s="4"/>
-      <c r="Q29" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q29" s="4"/>
       <c r="R29" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S29" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S29" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" s="4"/>
       <c r="B30" s="6"/>
       <c r="C30" s="8" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -1637,27 +1708,29 @@
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
       <c r="L30" s="4" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="M30" s="4"/>
-      <c r="N30" s="4">
-        <v>1</v>
-      </c>
-      <c r="O30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4">
+        <v>1</v>
+      </c>
       <c r="P30" s="4"/>
-      <c r="Q30" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="Q30" s="4"/>
       <c r="R30" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="S30" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="S30" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
-    </row>
-    <row r="33" spans="1:21" customHeight="1" ht="5">
+      <c r="V30" s="4"/>
+      <c r="W30" s="4"/>
+    </row>
+    <row r="33" spans="1:23" customHeight="1" ht="5">
       <c r="A33" s="10" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -1679,6 +1752,8 @@
       <c r="S33" s="10"/>
       <c r="T33" s="10"/>
       <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>